<commit_message>
Add in Marlin V1.1.6
Copying across Marlin for configuration
</commit_message>
<xml_diff>
--- a/logs/calibration analysis.xlsx
+++ b/logs/calibration analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Nominal</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Z-0.2mm line (diag)</t>
+  </si>
+  <si>
+    <t>z 2017-10-11 after fixing x carriage</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -235,7 +237,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.11951224846894144"/>
+                  <c:x val="0.11951224846894147"/>
                   <c:y val="0.26999489647127445"/>
                 </c:manualLayout>
               </c:layout>
@@ -279,23 +281,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="92628096"/>
-        <c:axId val="92630016"/>
+        <c:axId val="90288896"/>
+        <c:axId val="90290432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92628096"/>
+        <c:axId val="90288896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92630016"/>
+        <c:crossAx val="90290432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92630016"/>
+        <c:axId val="90290432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -303,20 +305,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92628096"/>
+        <c:crossAx val="90288896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -452,30 +453,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102975744"/>
-        <c:axId val="102984320"/>
+        <c:axId val="93231744"/>
+        <c:axId val="93245824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102975744"/>
+        <c:axId val="93231744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102984320"/>
+        <c:crossAx val="93245824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102984320"/>
+        <c:axId val="93245824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102975744"/>
+        <c:crossAx val="93231744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -488,7 +489,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -531,7 +532,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18876507790249628"/>
+                  <c:x val="-0.18876507790249633"/>
                   <c:y val="1.0198625702291192E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -623,30 +624,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="86573056"/>
-        <c:axId val="86574592"/>
+        <c:axId val="93946624"/>
+        <c:axId val="93948160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86573056"/>
+        <c:axId val="93946624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86574592"/>
+        <c:crossAx val="93948160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86574592"/>
+        <c:axId val="93948160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86573056"/>
+        <c:crossAx val="93946624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -659,7 +660,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -717,7 +718,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18876507790249639"/>
+                  <c:x val="-0.18876507790249644"/>
                   <c:y val="1.0198625702291192E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -809,30 +810,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91760512"/>
-        <c:axId val="91762048"/>
+        <c:axId val="94116480"/>
+        <c:axId val="94138752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91760512"/>
+        <c:axId val="94116480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91762048"/>
+        <c:crossAx val="94138752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91762048"/>
+        <c:axId val="94138752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91760512"/>
+        <c:crossAx val="94116480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -845,7 +846,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -888,8 +889,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.7630675154967331E-3"/>
-                  <c:y val="-5.7164936611040331E-3"/>
+                  <c:x val="1.7630675154967335E-3"/>
+                  <c:y val="-5.7164936611040348E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -986,30 +987,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="104387712"/>
-        <c:axId val="104389248"/>
+        <c:axId val="94159616"/>
+        <c:axId val="94161152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104387712"/>
+        <c:axId val="94159616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104389248"/>
+        <c:crossAx val="94161152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104389248"/>
+        <c:axId val="94161152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104387712"/>
+        <c:crossAx val="94159616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1022,7 +1023,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1566,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1587,6 +1588,9 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
       <c r="Z4" t="s">
         <v>9</v>
       </c>
@@ -1607,6 +1611,9 @@
       <c r="C5">
         <v>4.3499999999999996</v>
       </c>
+      <c r="D5">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="Z5" t="s">
         <v>12</v>
       </c>
@@ -1628,6 +1635,9 @@
       <c r="C6">
         <v>9.3000000000000007</v>
       </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:28">
       <c r="A7">
@@ -1639,6 +1649,9 @@
       <c r="C7">
         <v>14.3</v>
       </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:28">
       <c r="A8">
@@ -1650,6 +1663,9 @@
       <c r="C8">
         <v>19.3</v>
       </c>
+      <c r="D8">
+        <v>19.95</v>
+      </c>
     </row>
     <row r="9" spans="1:28">
       <c r="A9">
@@ -1661,6 +1677,9 @@
       <c r="C9">
         <v>24.35</v>
       </c>
+      <c r="D9">
+        <v>24.95</v>
+      </c>
     </row>
     <row r="10" spans="1:28">
       <c r="A10">
@@ -1672,6 +1691,9 @@
       <c r="C10">
         <v>29.3</v>
       </c>
+      <c r="D10">
+        <v>29.95</v>
+      </c>
     </row>
     <row r="11" spans="1:28">
       <c r="A11">
@@ -1683,6 +1705,9 @@
       <c r="C11">
         <v>34.4</v>
       </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:28">
       <c r="A12">
@@ -1694,6 +1719,9 @@
       <c r="C12">
         <v>39.35</v>
       </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:28">
       <c r="A13">
@@ -1705,6 +1733,9 @@
       <c r="C13">
         <v>44.4</v>
       </c>
+      <c r="D13">
+        <v>44.95</v>
+      </c>
     </row>
     <row r="14" spans="1:28">
       <c r="A14">
@@ -1716,6 +1747,9 @@
       <c r="C14">
         <v>49.3</v>
       </c>
+      <c r="D14">
+        <v>49.95</v>
+      </c>
     </row>
     <row r="15" spans="1:28">
       <c r="A15">
@@ -1727,6 +1761,9 @@
       <c r="C15">
         <v>54.35</v>
       </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:28">
       <c r="A16">
@@ -1738,8 +1775,11 @@
       <c r="C16">
         <v>59.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D16">
+        <v>59.95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1751,8 +1791,12 @@
         <f>SLOPE(C5:C16,$A$5:$A$16)</f>
         <v>1.0003496503496503</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="2">
+        <f>SLOPE(D5:D16,$A$5:$A$16)</f>
+        <v>0.99874125874125874</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1764,8 +1808,12 @@
         <f>INTERCEPT(C5:C16, $A$5:$A$16)</f>
         <v>-0.67803030303030098</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D19">
+        <f>INTERCEPT(D5:D16, $A$5:$A$16)</f>
+        <v>2.4242424242416405E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1773,7 +1821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>5</v>
       </c>
@@ -1781,7 +1829,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>10</v>
       </c>
@@ -1789,7 +1837,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1797,7 +1845,7 @@
         <v>15.15</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1805,7 +1853,7 @@
         <v>20.149999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1813,7 +1861,7 @@
         <v>25.15</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>30</v>
       </c>
@@ -1821,7 +1869,7 @@
         <v>30.1</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>35</v>
       </c>
@@ -1829,7 +1877,7 @@
         <v>35.25</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>40</v>
       </c>
@@ -1837,7 +1885,7 @@
         <v>40.35</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>45</v>
       </c>
@@ -1845,7 +1893,7 @@
         <v>45.2</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>50</v>
       </c>
@@ -1853,7 +1901,7 @@
         <v>50.45</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Adjustments to M92 E
Adjusted extruder steps per unit based on experiments
</commit_message>
<xml_diff>
--- a/logs/calibration analysis.xlsx
+++ b/logs/calibration analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="310" windowWidth="15060" windowHeight="7060" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="310" windowWidth="15060" windowHeight="7060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2017-10-05" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
   <si>
     <t>Nominal</t>
   </si>
@@ -88,6 +88,165 @@
   </si>
   <si>
     <t>z 2017-10-11 after fixing x carriage</t>
+  </si>
+  <si>
+    <t>Extruder calculation</t>
+  </si>
+  <si>
+    <t>e_steps_per_mm = (motor_steps_per_rev * driver_microstep) * (big_gear_teeth / small_gear_teeth) / (hob_effective_diameter * pi)</t>
+  </si>
+  <si>
+    <t>From Triffid Hunter's Calibration Guide</t>
+  </si>
+  <si>
+    <t>Motor steps per rev</t>
+  </si>
+  <si>
+    <t>Driver microstep</t>
+  </si>
+  <si>
+    <t>Big gear teeth</t>
+  </si>
+  <si>
+    <t>Small gear teeth</t>
+  </si>
+  <si>
+    <t>Hob Diameter</t>
+  </si>
+  <si>
+    <t>The values for the X and Y axis are calculated using the following formula:</t>
+  </si>
+  <si>
+    <t>DEFAULT_AXIS_STEPS_PER_UNIT = (Steps per rotation * Microsteps per step) / ( Pulley teeth * Belt</t>
+  </si>
+  <si>
+    <t>pitch). The stepper motors supplied with the kit are 1.8 degree/step motors, which is 200 steps per</t>
+  </si>
+  <si>
+    <t>revolution, and 1/16th microsteps. The pulleys are 14 teeth and the belt pitch is 2.5mm. Thus this figure</t>
+  </si>
+  <si>
+    <t>(200*16)/(14*2.5)=91.4286. If you wish to use 16 teeth pulleys, for example, the figure becomes</t>
+  </si>
+  <si>
+    <t>(200*16)/(16*2.5)=80.</t>
+  </si>
+  <si>
+    <t>Steps per mm</t>
+  </si>
+  <si>
+    <t>Observed</t>
+  </si>
+  <si>
+    <t>With 9 teeth (visible in old instructions)</t>
+  </si>
+  <si>
+    <t>In firmware</t>
+  </si>
+  <si>
+    <t>Extrusion test</t>
+  </si>
+  <si>
+    <t>Requested extrusion</t>
+  </si>
+  <si>
+    <t>Start postiion</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Actual extrusion</t>
+  </si>
+  <si>
+    <t>Scaling factor</t>
+  </si>
+  <si>
+    <t>New steps per mm</t>
+  </si>
+  <si>
+    <t>Implied diameter</t>
+  </si>
+  <si>
+    <t>Measured diameter of hobbed bolt as 5.35mm</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Extruding</t>
+  </si>
+  <si>
+    <t>Not at extruder, after loosening and retightening bolts</t>
+  </si>
+  <si>
+    <t>There is no change in extruded length - some max value reached due to speed?</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Tighten bolts to height of 12.6/12.3</t>
+  </si>
+  <si>
+    <t>Slipping observed</t>
+  </si>
+  <si>
+    <t>Loosened to 14.49/15 (finger tight)</t>
+  </si>
+  <si>
+    <t>+tight feed</t>
+  </si>
+  <si>
+    <t>+loose feed</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>G1 X139.957 Y2.500 E7.10147</t>
+  </si>
+  <si>
+    <t>G1 X139.957 Y137.500 E12.23232</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>Feed assumed at</t>
+  </si>
+  <si>
+    <t>y travel</t>
+  </si>
+  <si>
+    <t>Time (minutes)</t>
+  </si>
+  <si>
+    <t>Time (seconds)</t>
+  </si>
+  <si>
+    <t>e travel</t>
+  </si>
+  <si>
+    <t>e feed</t>
+  </si>
+  <si>
+    <t>No gaps</t>
+  </si>
+  <si>
+    <t>No gaps visible</t>
+  </si>
+  <si>
+    <t>Can see gaps</t>
   </si>
 </sst>
 </file>
@@ -97,7 +256,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,16 +264,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,14 +293,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FF2F6FAB"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FF2F6FAB"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FF2F6FAB"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FF2F6FAB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,7 +432,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.11951224846894147"/>
+                  <c:x val="0.1195122484689415"/>
                   <c:y val="0.26999489647127445"/>
                 </c:manualLayout>
               </c:layout>
@@ -281,23 +476,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="90288896"/>
-        <c:axId val="90290432"/>
+        <c:axId val="96125696"/>
+        <c:axId val="96127232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90288896"/>
+        <c:axId val="96125696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90290432"/>
+        <c:crossAx val="96127232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90290432"/>
+        <c:axId val="96127232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -305,7 +500,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90288896"/>
+        <c:crossAx val="96125696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -317,7 +512,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -453,30 +648,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93231744"/>
-        <c:axId val="93245824"/>
+        <c:axId val="93456256"/>
+        <c:axId val="93457792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93231744"/>
+        <c:axId val="93456256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93245824"/>
+        <c:crossAx val="93457792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93245824"/>
+        <c:axId val="93457792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93231744"/>
+        <c:crossAx val="93456256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -489,7 +684,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -532,7 +727,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18876507790249633"/>
+                  <c:x val="-0.18876507790249639"/>
                   <c:y val="1.0198625702291192E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -624,30 +819,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93946624"/>
-        <c:axId val="93948160"/>
+        <c:axId val="93519872"/>
+        <c:axId val="93521408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93946624"/>
+        <c:axId val="93519872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93948160"/>
+        <c:crossAx val="93521408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93948160"/>
+        <c:axId val="93521408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93946624"/>
+        <c:crossAx val="93519872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -660,7 +855,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -718,7 +913,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18876507790249644"/>
+                  <c:x val="-0.18876507790249647"/>
                   <c:y val="1.0198625702291192E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -810,30 +1005,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="94116480"/>
-        <c:axId val="94138752"/>
+        <c:axId val="93579136"/>
+        <c:axId val="93580672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94116480"/>
+        <c:axId val="93579136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94138752"/>
+        <c:crossAx val="93580672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94138752"/>
+        <c:axId val="93580672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94116480"/>
+        <c:crossAx val="93579136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -846,7 +1041,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -889,8 +1084,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.7630675154967335E-3"/>
-                  <c:y val="-5.7164936611040348E-3"/>
+                  <c:x val="1.7630675154967339E-3"/>
+                  <c:y val="-5.7164936611040374E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -987,30 +1182,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="94159616"/>
-        <c:axId val="94161152"/>
+        <c:axId val="94154752"/>
+        <c:axId val="94156288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94159616"/>
+        <c:axId val="94154752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94161152"/>
+        <c:crossAx val="94156288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94161152"/>
+        <c:axId val="94156288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94159616"/>
+        <c:crossAx val="94154752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1023,7 +1218,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1567,7 +1762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -2150,12 +2345,985 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N57" sqref="N57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1"/>
+    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="A3" s="3"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.5">
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>53</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>5.35</v>
+      </c>
+      <c r="G9" s="6">
+        <f>B9*C9*(D9/E9)/(F9*PI())</f>
+        <v>917.33826162737307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>53</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>5.35</v>
+      </c>
+      <c r="G10" s="6">
+        <f>B10*C10*(D10/E10)/(F10*PI())</f>
+        <v>1121.1912086556781</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>200</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>53</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6">
+        <f>((B11*C11)*(D11/E11))/G11/PI()</f>
+        <v>4.6911774205542951</v>
+      </c>
+      <c r="G11">
+        <v>1046.1679999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <v>200</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>53</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" s="6">
+        <f>((B12*C12)*(D12/E12))/G12/PI()</f>
+        <v>5.3345214127243974</v>
+      </c>
+      <c r="G12">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="F13">
+        <f>((B12*C12)*(D12/E12))/PI()</f>
+        <v>4907.7596997064456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="K29" t="s">
+        <v>57</v>
+      </c>
+      <c r="L29" t="s">
+        <v>59</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>920</v>
+      </c>
+      <c r="C30">
+        <v>920</v>
+      </c>
+      <c r="D30">
+        <v>920</v>
+      </c>
+      <c r="E30">
+        <v>920</v>
+      </c>
+      <c r="F30">
+        <v>1028</v>
+      </c>
+      <c r="G30">
+        <v>1028</v>
+      </c>
+      <c r="H30">
+        <v>1028</v>
+      </c>
+      <c r="I30">
+        <v>1028</v>
+      </c>
+      <c r="J30">
+        <v>1028</v>
+      </c>
+      <c r="K30">
+        <v>1028</v>
+      </c>
+      <c r="L30">
+        <v>1028</v>
+      </c>
+      <c r="M30">
+        <v>1028</v>
+      </c>
+      <c r="N30">
+        <v>1028</v>
+      </c>
+      <c r="O30">
+        <v>920</v>
+      </c>
+      <c r="P30">
+        <v>1230</v>
+      </c>
+      <c r="Q30">
+        <v>1230</v>
+      </c>
+      <c r="R30">
+        <v>1230</v>
+      </c>
+      <c r="S30">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31">
+        <v>10</v>
+      </c>
+      <c r="I31">
+        <v>300</v>
+      </c>
+      <c r="J31">
+        <v>600</v>
+      </c>
+      <c r="K31">
+        <v>600</v>
+      </c>
+      <c r="L31">
+        <v>600</v>
+      </c>
+      <c r="M31">
+        <v>300</v>
+      </c>
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31">
+        <v>100</v>
+      </c>
+      <c r="P31">
+        <v>100</v>
+      </c>
+      <c r="Q31">
+        <v>50</v>
+      </c>
+      <c r="R31">
+        <v>100</v>
+      </c>
+      <c r="S31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32">
+        <v>100</v>
+      </c>
+      <c r="C32">
+        <v>100</v>
+      </c>
+      <c r="D32">
+        <v>100</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+      <c r="G32">
+        <v>100</v>
+      </c>
+      <c r="H32">
+        <v>100</v>
+      </c>
+      <c r="I32">
+        <v>100</v>
+      </c>
+      <c r="J32">
+        <v>100</v>
+      </c>
+      <c r="K32">
+        <v>100</v>
+      </c>
+      <c r="L32">
+        <v>100</v>
+      </c>
+      <c r="M32">
+        <v>100</v>
+      </c>
+      <c r="N32">
+        <v>100</v>
+      </c>
+      <c r="O32">
+        <v>100</v>
+      </c>
+      <c r="P32">
+        <v>100</v>
+      </c>
+      <c r="Q32">
+        <v>100</v>
+      </c>
+      <c r="R32">
+        <v>100</v>
+      </c>
+      <c r="S32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33">
+        <v>124.9</v>
+      </c>
+      <c r="C33">
+        <v>119.98</v>
+      </c>
+      <c r="D33">
+        <v>120.22</v>
+      </c>
+      <c r="E33">
+        <v>120.37</v>
+      </c>
+      <c r="F33">
+        <v>120.37</v>
+      </c>
+      <c r="G33">
+        <v>120.45</v>
+      </c>
+      <c r="H33">
+        <v>120.54</v>
+      </c>
+      <c r="I33">
+        <v>120.64</v>
+      </c>
+      <c r="J33">
+        <v>120.57</v>
+      </c>
+      <c r="K33">
+        <v>120.52</v>
+      </c>
+      <c r="L33">
+        <v>120</v>
+      </c>
+      <c r="M33">
+        <v>120</v>
+      </c>
+      <c r="N33">
+        <v>120.27</v>
+      </c>
+      <c r="O33">
+        <v>120.22</v>
+      </c>
+      <c r="P33">
+        <v>120.43</v>
+      </c>
+      <c r="Q33">
+        <v>120.37</v>
+      </c>
+      <c r="R33">
+        <v>119.64</v>
+      </c>
+      <c r="S33">
+        <v>120.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>36.96</v>
+      </c>
+      <c r="C34">
+        <v>18.95</v>
+      </c>
+      <c r="D34">
+        <v>29.3</v>
+      </c>
+      <c r="E34">
+        <v>30.86</v>
+      </c>
+      <c r="F34">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="G34">
+        <v>36.68</v>
+      </c>
+      <c r="H34">
+        <v>37.24</v>
+      </c>
+      <c r="I34">
+        <v>55.09</v>
+      </c>
+      <c r="J34">
+        <v>25.27</v>
+      </c>
+      <c r="K34">
+        <v>89.04</v>
+      </c>
+      <c r="L34">
+        <v>87.37</v>
+      </c>
+      <c r="N34">
+        <v>37.020000000000003</v>
+      </c>
+      <c r="O34">
+        <v>45.3</v>
+      </c>
+      <c r="P34">
+        <v>21.12</v>
+      </c>
+      <c r="Q34">
+        <v>20.48</v>
+      </c>
+      <c r="R34">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="S34">
+        <v>20.98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <f>B33-B34</f>
+        <v>87.94</v>
+      </c>
+      <c r="C35">
+        <f>C33-C34</f>
+        <v>101.03</v>
+      </c>
+      <c r="D35">
+        <f>D33-D34</f>
+        <v>90.92</v>
+      </c>
+      <c r="E35">
+        <f>E33-E34</f>
+        <v>89.51</v>
+      </c>
+      <c r="F35">
+        <f>F33-F34</f>
+        <v>86.570000000000007</v>
+      </c>
+      <c r="G35">
+        <f>G33-G34</f>
+        <v>83.77000000000001</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ref="H35:S35" si="0">H33-H34</f>
+        <v>83.300000000000011</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>65.55</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>95.3</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>31.47999999999999</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>32.629999999999995</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>83.25</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="0"/>
+        <v>74.92</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>99.31</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="0"/>
+        <v>99.89</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="0"/>
+        <v>99.38</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="0"/>
+        <v>99.039999999999992</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="5">
+        <f>B32/B35</f>
+        <v>1.1371389583807141</v>
+      </c>
+      <c r="C36" s="5">
+        <f>C32/C35</f>
+        <v>0.98980500841334251</v>
+      </c>
+      <c r="D36" s="5">
+        <f>D32/D35</f>
+        <v>1.0998680158380993</v>
+      </c>
+      <c r="E36" s="5">
+        <f>E32/E35</f>
+        <v>1.1171936096525528</v>
+      </c>
+      <c r="F36" s="5">
+        <f>F32/F35</f>
+        <v>1.1551345731777751</v>
+      </c>
+      <c r="G36" s="5">
+        <f>G32/G35</f>
+        <v>1.1937447773665988</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" ref="H36:S36" si="1">H32/H35</f>
+        <v>1.2004801920768307</v>
+      </c>
+      <c r="I36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.5255530129672006</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0493179433368311</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" si="1"/>
+        <v>3.176620076238883</v>
+      </c>
+      <c r="L36" s="5">
+        <f t="shared" si="1"/>
+        <v>3.064664419246093</v>
+      </c>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2012012012012012</v>
+      </c>
+      <c r="O36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3347570742124932</v>
+      </c>
+      <c r="P36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.006947940791461</v>
+      </c>
+      <c r="Q36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0011012113324658</v>
+      </c>
+      <c r="R36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0062386798148522</v>
+      </c>
+      <c r="S36" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0096930533117934</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37">
+        <f>B30*B36</f>
+        <v>1046.1678417102569</v>
+      </c>
+      <c r="C37">
+        <f>C30*C36</f>
+        <v>910.62060774027509</v>
+      </c>
+      <c r="D37">
+        <f>D30*D36</f>
+        <v>1011.8785745710514</v>
+      </c>
+      <c r="E37">
+        <f>E30*E36</f>
+        <v>1027.8181208803485</v>
+      </c>
+      <c r="F37">
+        <f>F30*F36</f>
+        <v>1187.4783412267527</v>
+      </c>
+      <c r="G37">
+        <f>G30*G36</f>
+        <v>1227.1696311328635</v>
+      </c>
+      <c r="H37">
+        <f t="shared" ref="H37:S37" si="2">H30*H36</f>
+        <v>1234.0936374549819</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>1568.2684973302821</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>1078.6988457502625</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="2"/>
+        <v>3265.5654383735719</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>3150.4750229849838</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>1234.834834834835</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="2"/>
+        <v>1227.9765082754939</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="2"/>
+        <v>1238.545967173497</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="2"/>
+        <v>1231.3544899389328</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="2"/>
+        <v>1237.6735761722682</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="2"/>
+        <v>1241.9224555735059</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38">
+        <f>4907.76/B37</f>
+        <v>4.6911784173913054</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ref="C38:S38" si="3">4907.76/C37</f>
+        <v>5.3894673130434789</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>4.8501471652173915</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>4.7749304086956528</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>4.132925906614787</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>3.9992515097276273</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>3.9768133073929963</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>3.1294131128404672</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>4.5497035797665362</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="3"/>
+        <v>1.5028821478599217</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="3"/>
+        <v>1.5577841322957195</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="3"/>
+        <v>3.9744262645914397</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="3"/>
+        <v>3.9966236869565219</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>3.9625174439024393</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="3"/>
+        <v>3.9856597268292684</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="3"/>
+        <v>3.9653104780487802</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="3"/>
+        <v>3.9517443121951215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="G39" t="s">
+        <v>54</v>
+      </c>
+      <c r="K39" t="s">
+        <v>58</v>
+      </c>
+      <c r="L39" t="s">
+        <v>58</v>
+      </c>
+      <c r="M39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="N48">
+        <v>1230</v>
+      </c>
+      <c r="O48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="N49">
+        <f>N48*0.995</f>
+        <v>1223.8499999999999</v>
+      </c>
+      <c r="O49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="N50">
+        <f>N49*0.995</f>
+        <v>1217.7307499999999</v>
+      </c>
+      <c r="O50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51">
+        <v>2.5</v>
+      </c>
+      <c r="N51">
+        <f>N50*0.995</f>
+        <v>1211.6420962499999</v>
+      </c>
+      <c r="O51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52">
+        <v>137.5</v>
+      </c>
+      <c r="N52">
+        <f>N51*0.995</f>
+        <v>1205.58388576875</v>
+      </c>
+      <c r="O52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53">
+        <v>7.1014699999999999</v>
+      </c>
+      <c r="N53">
+        <v>1100</v>
+      </c>
+      <c r="O53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54">
+        <v>12.23232</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56">
+        <f>B52-B51</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57">
+        <f>B56/B55</f>
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58">
+        <f>B57*60</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59">
+        <f>B54-B53</f>
+        <v>5.1308499999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60">
+        <f>B59/B57</f>
+        <v>45.60755555555555</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed extruder to new version
From https://github.com/reprappro/Extruder-drive
</commit_message>
<xml_diff>
--- a/logs/calibration analysis.xlsx
+++ b/logs/calibration analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>Nominal</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Can see gaps</t>
+  </si>
+  <si>
+    <t>BELOW IS ALL FOR OLD EXTRUDER DESIGN USED PRE 2017-11-09</t>
+  </si>
+  <si>
+    <t>On RepRapPro site</t>
   </si>
 </sst>
 </file>
@@ -256,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +275,14 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -312,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -325,6 +339,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +447,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.1195122484689415"/>
+                  <c:x val="0.11951224846894153"/>
                   <c:y val="0.26999489647127445"/>
                 </c:manualLayout>
               </c:layout>
@@ -476,23 +491,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="96125696"/>
-        <c:axId val="96127232"/>
+        <c:axId val="70984832"/>
+        <c:axId val="70986368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96125696"/>
+        <c:axId val="70984832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96127232"/>
+        <c:crossAx val="70986368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96127232"/>
+        <c:axId val="70986368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -500,7 +515,175 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96125696"/>
+        <c:crossAx val="70984832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2017-10-07'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>z (4000)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2017-10-07'!$A$5:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2017-10-07'!$B$5:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="71011328"/>
+        <c:axId val="71037696"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="71011328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71037696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="71037696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71011328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -518,185 +701,11 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2017-10-07'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>z (4000)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'2017-10-07'!$A$5:$A$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'2017-10-07'!$B$5:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29.1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>34.15</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>48.9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>53.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>58.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="93456256"/>
-        <c:axId val="93457792"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="93456256"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93457792"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="93457792"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93456256"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -727,7 +736,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18876507790249639"/>
+                  <c:x val="-0.18876507790249644"/>
                   <c:y val="1.0198625702291192E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -819,43 +828,42 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93519872"/>
-        <c:axId val="93521408"/>
+        <c:axId val="87528576"/>
+        <c:axId val="87530112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93519872"/>
+        <c:axId val="87528576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93521408"/>
+        <c:crossAx val="87530112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93521408"/>
+        <c:axId val="87530112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93519872"/>
+        <c:crossAx val="87528576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -881,7 +889,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -913,7 +920,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18876507790249647"/>
+                  <c:x val="-0.18876507790249653"/>
                   <c:y val="1.0198625702291192E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -1005,43 +1012,42 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93579136"/>
-        <c:axId val="93580672"/>
+        <c:axId val="95890432"/>
+        <c:axId val="95912704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93579136"/>
+        <c:axId val="95890432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93580672"/>
+        <c:crossAx val="95912704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93580672"/>
+        <c:axId val="95912704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93579136"/>
+        <c:crossAx val="95890432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1051,9 +1057,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1084,8 +1088,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.7630675154967339E-3"/>
-                  <c:y val="-5.7164936611040374E-3"/>
+                  <c:x val="1.7630675154967344E-3"/>
+                  <c:y val="-5.7164936611040391E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1182,43 +1186,42 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="94154752"/>
-        <c:axId val="94156288"/>
+        <c:axId val="95933568"/>
+        <c:axId val="95935104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94154752"/>
+        <c:axId val="95933568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94156288"/>
+        <c:crossAx val="95935104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94156288"/>
+        <c:axId val="95935104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94154752"/>
+        <c:crossAx val="95933568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2345,10 +2348,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S60"/>
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N57" sqref="N57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2361,964 +2364,1023 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1"/>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:7" ht="43.5">
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>78</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4">
+        <v>945</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="43.5">
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8">
+        <v>39</v>
+      </c>
+      <c r="B5">
         <v>200</v>
       </c>
-      <c r="C8">
+      <c r="C5">
         <v>16</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9">
-        <v>200</v>
-      </c>
-      <c r="C9">
-        <v>16</v>
-      </c>
-      <c r="D9">
+      <c r="D5">
         <v>53</v>
       </c>
-      <c r="E9">
+      <c r="E5">
         <v>11</v>
       </c>
-      <c r="F9">
+      <c r="F5">
         <v>5.35</v>
       </c>
-      <c r="G9" s="6">
-        <f>B9*C9*(D9/E9)/(F9*PI())</f>
+      <c r="G5" s="6">
+        <f>B5*C5*(D5/E5)/(F5*PI())</f>
         <v>917.33826162737307</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10">
-        <v>200</v>
-      </c>
-      <c r="C10">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>53</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>5.35</v>
-      </c>
-      <c r="G10" s="6">
-        <f>B10*C10*(D10/E10)/(F10*PI())</f>
-        <v>1121.1912086556781</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11">
-        <v>200</v>
-      </c>
-      <c r="C11">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>53</v>
-      </c>
-      <c r="E11">
-        <v>11</v>
-      </c>
-      <c r="F11" s="6">
-        <f>((B11*C11)*(D11/E11))/G11/PI()</f>
-        <v>4.6911774205542951</v>
-      </c>
-      <c r="G11">
-        <v>1046.1679999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12">
-        <v>200</v>
-      </c>
-      <c r="C12">
-        <v>16</v>
-      </c>
-      <c r="D12">
-        <v>53</v>
-      </c>
-      <c r="E12">
-        <v>11</v>
-      </c>
-      <c r="F12" s="6">
-        <f>((B12*C12)*(D12/E12))/G12/PI()</f>
-        <v>5.3345214127243974</v>
-      </c>
-      <c r="G12">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="F13">
-        <f>((B12*C12)*(D12/E12))/PI()</f>
-        <v>4907.7596997064456</v>
-      </c>
+    <row r="12" spans="1:7" ht="15" thickBot="1">
+      <c r="A12" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1">
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.5">
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>53</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>5.35</v>
+      </c>
+      <c r="G19" s="6">
+        <f>B19*C19*(D19/E19)/(F19*PI())</f>
+        <v>917.33826162737307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>53</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>5.35</v>
+      </c>
+      <c r="G20" s="6">
+        <f>B20*C20*(D20/E20)/(F20*PI())</f>
+        <v>1121.1912086556781</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21">
+        <v>200</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>53</v>
+      </c>
+      <c r="E21">
+        <v>11</v>
+      </c>
+      <c r="F21" s="6">
+        <f>((B21*C21)*(D21/E21))/G21/PI()</f>
+        <v>4.6911774205542951</v>
+      </c>
+      <c r="G21">
+        <v>1046.1679999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <v>200</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>53</v>
+      </c>
+      <c r="E22">
+        <v>11</v>
+      </c>
+      <c r="F22" s="6">
+        <f>((B22*C22)*(D22/E22))/G22/PI()</f>
+        <v>5.3345214127243974</v>
+      </c>
+      <c r="G22">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="F23">
+        <f>((B22*C22)*(D22/E22))/PI()</f>
+        <v>4907.7596997064456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
-      <c r="A20" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
-      <c r="A21" t="s">
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
-      <c r="A22" t="s">
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="K29" t="s">
-        <v>57</v>
-      </c>
-      <c r="L29" t="s">
-        <v>59</v>
-      </c>
-      <c r="R29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="S29" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19">
-      <c r="A30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30">
-        <v>920</v>
-      </c>
-      <c r="C30">
-        <v>920</v>
-      </c>
-      <c r="D30">
-        <v>920</v>
-      </c>
-      <c r="E30">
-        <v>920</v>
-      </c>
-      <c r="F30">
-        <v>1028</v>
-      </c>
-      <c r="G30">
-        <v>1028</v>
-      </c>
-      <c r="H30">
-        <v>1028</v>
-      </c>
-      <c r="I30">
-        <v>1028</v>
-      </c>
-      <c r="J30">
-        <v>1028</v>
-      </c>
-      <c r="K30">
-        <v>1028</v>
-      </c>
-      <c r="L30">
-        <v>1028</v>
-      </c>
-      <c r="M30">
-        <v>1028</v>
-      </c>
-      <c r="N30">
-        <v>1028</v>
-      </c>
-      <c r="O30">
-        <v>920</v>
-      </c>
-      <c r="P30">
-        <v>1230</v>
-      </c>
-      <c r="Q30">
-        <v>1230</v>
-      </c>
-      <c r="R30">
-        <v>1230</v>
-      </c>
-      <c r="S30">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19">
-      <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" t="s">
-        <v>56</v>
-      </c>
-      <c r="H31">
-        <v>10</v>
-      </c>
-      <c r="I31">
-        <v>300</v>
-      </c>
-      <c r="J31">
-        <v>600</v>
-      </c>
-      <c r="K31">
-        <v>600</v>
-      </c>
-      <c r="L31">
-        <v>600</v>
-      </c>
-      <c r="M31">
-        <v>300</v>
-      </c>
-      <c r="N31">
-        <v>100</v>
-      </c>
-      <c r="O31">
-        <v>100</v>
-      </c>
-      <c r="P31">
-        <v>100</v>
-      </c>
-      <c r="Q31">
-        <v>50</v>
-      </c>
-      <c r="R31">
-        <v>100</v>
-      </c>
-      <c r="S31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19">
-      <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32">
-        <v>100</v>
-      </c>
-      <c r="C32">
-        <v>100</v>
-      </c>
-      <c r="D32">
-        <v>100</v>
-      </c>
-      <c r="E32">
-        <v>100</v>
-      </c>
-      <c r="F32">
-        <v>100</v>
-      </c>
-      <c r="G32">
-        <v>100</v>
-      </c>
-      <c r="H32">
-        <v>100</v>
-      </c>
-      <c r="I32">
-        <v>100</v>
-      </c>
-      <c r="J32">
-        <v>100</v>
-      </c>
-      <c r="K32">
-        <v>100</v>
-      </c>
-      <c r="L32">
-        <v>100</v>
-      </c>
-      <c r="M32">
-        <v>100</v>
-      </c>
-      <c r="N32">
-        <v>100</v>
-      </c>
-      <c r="O32">
-        <v>100</v>
-      </c>
-      <c r="P32">
-        <v>100</v>
-      </c>
-      <c r="Q32">
-        <v>100</v>
-      </c>
-      <c r="R32">
-        <v>100</v>
-      </c>
-      <c r="S32">
-        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:19">
       <c r="A33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33">
-        <v>124.9</v>
-      </c>
-      <c r="C33">
-        <v>119.98</v>
-      </c>
-      <c r="D33">
-        <v>120.22</v>
-      </c>
-      <c r="E33">
-        <v>120.37</v>
-      </c>
-      <c r="F33">
-        <v>120.37</v>
-      </c>
-      <c r="G33">
-        <v>120.45</v>
-      </c>
-      <c r="H33">
-        <v>120.54</v>
-      </c>
-      <c r="I33">
-        <v>120.64</v>
-      </c>
-      <c r="J33">
-        <v>120.57</v>
-      </c>
-      <c r="K33">
-        <v>120.52</v>
-      </c>
-      <c r="L33">
-        <v>120</v>
-      </c>
-      <c r="M33">
-        <v>120</v>
-      </c>
-      <c r="N33">
-        <v>120.27</v>
-      </c>
-      <c r="O33">
-        <v>120.22</v>
-      </c>
-      <c r="P33">
-        <v>120.43</v>
-      </c>
-      <c r="Q33">
-        <v>120.37</v>
-      </c>
-      <c r="R33">
-        <v>119.64</v>
-      </c>
-      <c r="S33">
-        <v>120.02</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34">
-        <v>36.96</v>
-      </c>
-      <c r="C34">
-        <v>18.95</v>
-      </c>
-      <c r="D34">
-        <v>29.3</v>
-      </c>
-      <c r="E34">
-        <v>30.86</v>
-      </c>
-      <c r="F34">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="G34">
-        <v>36.68</v>
-      </c>
-      <c r="H34">
-        <v>37.24</v>
-      </c>
-      <c r="I34">
-        <v>55.09</v>
-      </c>
-      <c r="J34">
-        <v>25.27</v>
-      </c>
-      <c r="K34">
-        <v>89.04</v>
-      </c>
-      <c r="L34">
-        <v>87.37</v>
-      </c>
-      <c r="N34">
-        <v>37.020000000000003</v>
-      </c>
-      <c r="O34">
-        <v>45.3</v>
-      </c>
-      <c r="P34">
-        <v>21.12</v>
-      </c>
-      <c r="Q34">
-        <v>20.48</v>
-      </c>
-      <c r="R34">
-        <v>20.260000000000002</v>
-      </c>
-      <c r="S34">
-        <v>20.98</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35">
-        <f>B33-B34</f>
-        <v>87.94</v>
-      </c>
-      <c r="C35">
-        <f>C33-C34</f>
-        <v>101.03</v>
-      </c>
-      <c r="D35">
-        <f>D33-D34</f>
-        <v>90.92</v>
-      </c>
-      <c r="E35">
-        <f>E33-E34</f>
-        <v>89.51</v>
-      </c>
-      <c r="F35">
-        <f>F33-F34</f>
-        <v>86.570000000000007</v>
-      </c>
-      <c r="G35">
-        <f>G33-G34</f>
-        <v>83.77000000000001</v>
-      </c>
-      <c r="H35">
-        <f t="shared" ref="H35:S35" si="0">H33-H34</f>
-        <v>83.300000000000011</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="0"/>
-        <v>65.55</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="0"/>
-        <v>95.3</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="0"/>
-        <v>31.47999999999999</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="0"/>
-        <v>32.629999999999995</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="0"/>
-        <v>83.25</v>
-      </c>
-      <c r="O35">
-        <f t="shared" si="0"/>
-        <v>74.92</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="0"/>
-        <v>99.31</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="0"/>
-        <v>99.89</v>
-      </c>
-      <c r="R35">
-        <f t="shared" si="0"/>
-        <v>99.38</v>
-      </c>
-      <c r="S35">
-        <f t="shared" si="0"/>
-        <v>99.039999999999992</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19">
-      <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="5">
-        <f>B32/B35</f>
-        <v>1.1371389583807141</v>
-      </c>
-      <c r="C36" s="5">
-        <f>C32/C35</f>
-        <v>0.98980500841334251</v>
-      </c>
-      <c r="D36" s="5">
-        <f>D32/D35</f>
-        <v>1.0998680158380993</v>
-      </c>
-      <c r="E36" s="5">
-        <f>E32/E35</f>
-        <v>1.1171936096525528</v>
-      </c>
-      <c r="F36" s="5">
-        <f>F32/F35</f>
-        <v>1.1551345731777751</v>
-      </c>
-      <c r="G36" s="5">
-        <f>G32/G35</f>
-        <v>1.1937447773665988</v>
-      </c>
-      <c r="H36" s="5">
-        <f t="shared" ref="H36:S36" si="1">H32/H35</f>
-        <v>1.2004801920768307</v>
-      </c>
-      <c r="I36" s="5">
-        <f t="shared" si="1"/>
-        <v>1.5255530129672006</v>
-      </c>
-      <c r="J36" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0493179433368311</v>
-      </c>
-      <c r="K36" s="5">
-        <f t="shared" si="1"/>
-        <v>3.176620076238883</v>
-      </c>
-      <c r="L36" s="5">
-        <f t="shared" si="1"/>
-        <v>3.064664419246093</v>
-      </c>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5">
-        <f t="shared" si="1"/>
-        <v>1.2012012012012012</v>
-      </c>
-      <c r="O36" s="5">
-        <f t="shared" si="1"/>
-        <v>1.3347570742124932</v>
-      </c>
-      <c r="P36" s="5">
-        <f t="shared" si="1"/>
-        <v>1.006947940791461</v>
-      </c>
-      <c r="Q36" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0011012113324658</v>
-      </c>
-      <c r="R36" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0062386798148522</v>
-      </c>
-      <c r="S36" s="5">
-        <f t="shared" si="1"/>
-        <v>1.0096930533117934</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19">
-      <c r="A37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37">
-        <f>B30*B36</f>
-        <v>1046.1678417102569</v>
-      </c>
-      <c r="C37">
-        <f>C30*C36</f>
-        <v>910.62060774027509</v>
-      </c>
-      <c r="D37">
-        <f>D30*D36</f>
-        <v>1011.8785745710514</v>
-      </c>
-      <c r="E37">
-        <f>E30*E36</f>
-        <v>1027.8181208803485</v>
-      </c>
-      <c r="F37">
-        <f>F30*F36</f>
-        <v>1187.4783412267527</v>
-      </c>
-      <c r="G37">
-        <f>G30*G36</f>
-        <v>1227.1696311328635</v>
-      </c>
-      <c r="H37">
-        <f t="shared" ref="H37:S37" si="2">H30*H36</f>
-        <v>1234.0936374549819</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="2"/>
-        <v>1568.2684973302821</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="2"/>
-        <v>1078.6988457502625</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="2"/>
-        <v>3265.5654383735719</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="2"/>
-        <v>3150.4750229849838</v>
-      </c>
-      <c r="N37">
-        <f t="shared" si="2"/>
-        <v>1234.834834834835</v>
-      </c>
-      <c r="O37">
-        <f t="shared" si="2"/>
-        <v>1227.9765082754939</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="2"/>
-        <v>1238.545967173497</v>
-      </c>
-      <c r="Q37">
-        <f t="shared" si="2"/>
-        <v>1231.3544899389328</v>
-      </c>
-      <c r="R37">
-        <f t="shared" si="2"/>
-        <v>1237.6735761722682</v>
-      </c>
-      <c r="S37">
-        <f t="shared" si="2"/>
-        <v>1241.9224555735059</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:19">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B38">
-        <f>4907.76/B37</f>
-        <v>4.6911784173913054</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <f t="shared" ref="C38:S38" si="3">4907.76/C37</f>
-        <v>5.3894673130434789</v>
+        <v>2</v>
       </c>
       <c r="D38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+      <c r="K39" t="s">
+        <v>57</v>
+      </c>
+      <c r="L39" t="s">
+        <v>59</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>920</v>
+      </c>
+      <c r="C40">
+        <v>920</v>
+      </c>
+      <c r="D40">
+        <v>920</v>
+      </c>
+      <c r="E40">
+        <v>920</v>
+      </c>
+      <c r="F40">
+        <v>1028</v>
+      </c>
+      <c r="G40">
+        <v>1028</v>
+      </c>
+      <c r="H40">
+        <v>1028</v>
+      </c>
+      <c r="I40">
+        <v>1028</v>
+      </c>
+      <c r="J40">
+        <v>1028</v>
+      </c>
+      <c r="K40">
+        <v>1028</v>
+      </c>
+      <c r="L40">
+        <v>1028</v>
+      </c>
+      <c r="M40">
+        <v>1028</v>
+      </c>
+      <c r="N40">
+        <v>1028</v>
+      </c>
+      <c r="O40">
+        <v>920</v>
+      </c>
+      <c r="P40">
+        <v>1230</v>
+      </c>
+      <c r="Q40">
+        <v>1230</v>
+      </c>
+      <c r="R40">
+        <v>1230</v>
+      </c>
+      <c r="S40">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41">
+        <v>10</v>
+      </c>
+      <c r="I41">
+        <v>300</v>
+      </c>
+      <c r="J41">
+        <v>600</v>
+      </c>
+      <c r="K41">
+        <v>600</v>
+      </c>
+      <c r="L41">
+        <v>600</v>
+      </c>
+      <c r="M41">
+        <v>300</v>
+      </c>
+      <c r="N41">
+        <v>100</v>
+      </c>
+      <c r="O41">
+        <v>100</v>
+      </c>
+      <c r="P41">
+        <v>100</v>
+      </c>
+      <c r="Q41">
+        <v>50</v>
+      </c>
+      <c r="R41">
+        <v>100</v>
+      </c>
+      <c r="S41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>100</v>
+      </c>
+      <c r="C42">
+        <v>100</v>
+      </c>
+      <c r="D42">
+        <v>100</v>
+      </c>
+      <c r="E42">
+        <v>100</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+      <c r="G42">
+        <v>100</v>
+      </c>
+      <c r="H42">
+        <v>100</v>
+      </c>
+      <c r="I42">
+        <v>100</v>
+      </c>
+      <c r="J42">
+        <v>100</v>
+      </c>
+      <c r="K42">
+        <v>100</v>
+      </c>
+      <c r="L42">
+        <v>100</v>
+      </c>
+      <c r="M42">
+        <v>100</v>
+      </c>
+      <c r="N42">
+        <v>100</v>
+      </c>
+      <c r="O42">
+        <v>100</v>
+      </c>
+      <c r="P42">
+        <v>100</v>
+      </c>
+      <c r="Q42">
+        <v>100</v>
+      </c>
+      <c r="R42">
+        <v>100</v>
+      </c>
+      <c r="S42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>124.9</v>
+      </c>
+      <c r="C43">
+        <v>119.98</v>
+      </c>
+      <c r="D43">
+        <v>120.22</v>
+      </c>
+      <c r="E43">
+        <v>120.37</v>
+      </c>
+      <c r="F43">
+        <v>120.37</v>
+      </c>
+      <c r="G43">
+        <v>120.45</v>
+      </c>
+      <c r="H43">
+        <v>120.54</v>
+      </c>
+      <c r="I43">
+        <v>120.64</v>
+      </c>
+      <c r="J43">
+        <v>120.57</v>
+      </c>
+      <c r="K43">
+        <v>120.52</v>
+      </c>
+      <c r="L43">
+        <v>120</v>
+      </c>
+      <c r="M43">
+        <v>120</v>
+      </c>
+      <c r="N43">
+        <v>120.27</v>
+      </c>
+      <c r="O43">
+        <v>120.22</v>
+      </c>
+      <c r="P43">
+        <v>120.43</v>
+      </c>
+      <c r="Q43">
+        <v>120.37</v>
+      </c>
+      <c r="R43">
+        <v>119.64</v>
+      </c>
+      <c r="S43">
+        <v>120.02</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>36.96</v>
+      </c>
+      <c r="C44">
+        <v>18.95</v>
+      </c>
+      <c r="D44">
+        <v>29.3</v>
+      </c>
+      <c r="E44">
+        <v>30.86</v>
+      </c>
+      <c r="F44">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="G44">
+        <v>36.68</v>
+      </c>
+      <c r="H44">
+        <v>37.24</v>
+      </c>
+      <c r="I44">
+        <v>55.09</v>
+      </c>
+      <c r="J44">
+        <v>25.27</v>
+      </c>
+      <c r="K44">
+        <v>89.04</v>
+      </c>
+      <c r="L44">
+        <v>87.37</v>
+      </c>
+      <c r="N44">
+        <v>37.020000000000003</v>
+      </c>
+      <c r="O44">
+        <v>45.3</v>
+      </c>
+      <c r="P44">
+        <v>21.12</v>
+      </c>
+      <c r="Q44">
+        <v>20.48</v>
+      </c>
+      <c r="R44">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="S44">
+        <v>20.98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ref="B45:G45" si="0">B43-B44</f>
+        <v>87.94</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>101.03</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>90.92</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>89.51</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>86.570000000000007</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>83.77000000000001</v>
+      </c>
+      <c r="H45">
+        <f t="shared" ref="H45:S45" si="1">H43-H44</f>
+        <v>83.300000000000011</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>65.55</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>95.3</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>31.47999999999999</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="1"/>
+        <v>32.629999999999995</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="1"/>
+        <v>83.25</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="1"/>
+        <v>74.92</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="1"/>
+        <v>99.31</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="1"/>
+        <v>99.89</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="1"/>
+        <v>99.38</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="1"/>
+        <v>99.039999999999992</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="5">
+        <f t="shared" ref="B46:G46" si="2">B42/B45</f>
+        <v>1.1371389583807141</v>
+      </c>
+      <c r="C46" s="5">
+        <f t="shared" si="2"/>
+        <v>0.98980500841334251</v>
+      </c>
+      <c r="D46" s="5">
+        <f t="shared" si="2"/>
+        <v>1.0998680158380993</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1171936096525528</v>
+      </c>
+      <c r="F46" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1551345731777751</v>
+      </c>
+      <c r="G46" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1937447773665988</v>
+      </c>
+      <c r="H46" s="5">
+        <f t="shared" ref="H46:S46" si="3">H42/H45</f>
+        <v>1.2004801920768307</v>
+      </c>
+      <c r="I46" s="5">
         <f t="shared" si="3"/>
-        <v>4.8501471652173915</v>
-      </c>
-      <c r="E38">
+        <v>1.5255530129672006</v>
+      </c>
+      <c r="J46" s="5">
         <f t="shared" si="3"/>
-        <v>4.7749304086956528</v>
-      </c>
-      <c r="F38">
+        <v>1.0493179433368311</v>
+      </c>
+      <c r="K46" s="5">
         <f t="shared" si="3"/>
-        <v>4.132925906614787</v>
-      </c>
-      <c r="G38">
+        <v>3.176620076238883</v>
+      </c>
+      <c r="L46" s="5">
         <f t="shared" si="3"/>
-        <v>3.9992515097276273</v>
-      </c>
-      <c r="H38">
+        <v>3.064664419246093</v>
+      </c>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5">
         <f t="shared" si="3"/>
-        <v>3.9768133073929963</v>
-      </c>
-      <c r="I38">
+        <v>1.2012012012012012</v>
+      </c>
+      <c r="O46" s="5">
         <f t="shared" si="3"/>
-        <v>3.1294131128404672</v>
-      </c>
-      <c r="J38">
+        <v>1.3347570742124932</v>
+      </c>
+      <c r="P46" s="5">
         <f t="shared" si="3"/>
-        <v>4.5497035797665362</v>
-      </c>
-      <c r="K38">
+        <v>1.006947940791461</v>
+      </c>
+      <c r="Q46" s="5">
         <f t="shared" si="3"/>
-        <v>1.5028821478599217</v>
-      </c>
-      <c r="L38">
+        <v>1.0011012113324658</v>
+      </c>
+      <c r="R46" s="5">
         <f t="shared" si="3"/>
-        <v>1.5577841322957195</v>
-      </c>
-      <c r="N38">
+        <v>1.0062386798148522</v>
+      </c>
+      <c r="S46" s="5">
         <f t="shared" si="3"/>
-        <v>3.9744262645914397</v>
-      </c>
-      <c r="O38">
-        <f t="shared" si="3"/>
-        <v>3.9966236869565219</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="3"/>
-        <v>3.9625174439024393</v>
-      </c>
-      <c r="Q38">
-        <f t="shared" si="3"/>
-        <v>3.9856597268292684</v>
-      </c>
-      <c r="R38">
-        <f t="shared" si="3"/>
-        <v>3.9653104780487802</v>
-      </c>
-      <c r="S38">
-        <f t="shared" si="3"/>
-        <v>3.9517443121951215</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19">
-      <c r="G39" t="s">
-        <v>54</v>
-      </c>
-      <c r="K39" t="s">
-        <v>58</v>
-      </c>
-      <c r="L39" t="s">
-        <v>58</v>
-      </c>
-      <c r="M39" t="s">
-        <v>58</v>
+        <v>1.0096930533117934</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <f t="shared" ref="B47:G47" si="4">B40*B46</f>
+        <v>1046.1678417102569</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="4"/>
+        <v>910.62060774027509</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="4"/>
+        <v>1011.8785745710514</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="4"/>
+        <v>1027.8181208803485</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="4"/>
+        <v>1187.4783412267527</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="4"/>
+        <v>1227.1696311328635</v>
+      </c>
+      <c r="H47">
+        <f t="shared" ref="H47:S47" si="5">H40*H46</f>
+        <v>1234.0936374549819</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="5"/>
+        <v>1568.2684973302821</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="5"/>
+        <v>1078.6988457502625</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="5"/>
+        <v>3265.5654383735719</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="5"/>
+        <v>3150.4750229849838</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="5"/>
+        <v>1234.834834834835</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="5"/>
+        <v>1227.9765082754939</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="5"/>
+        <v>1238.545967173497</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="5"/>
+        <v>1231.3544899389328</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="5"/>
+        <v>1237.6735761722682</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="5"/>
+        <v>1241.9224555735059</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <f>4907.76/B47</f>
+        <v>4.6911784173913054</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48:S48" si="6">4907.76/C47</f>
+        <v>5.3894673130434789</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="6"/>
+        <v>4.8501471652173915</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>4.7749304086956528</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="6"/>
+        <v>4.132925906614787</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="6"/>
+        <v>3.9992515097276273</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="6"/>
+        <v>3.9768133073929963</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="6"/>
+        <v>3.1294131128404672</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="6"/>
+        <v>4.5497035797665362</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="6"/>
+        <v>1.5028821478599217</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="6"/>
+        <v>1.5577841322957195</v>
       </c>
       <c r="N48">
-        <v>1230</v>
-      </c>
-      <c r="O48" t="s">
-        <v>74</v>
+        <f t="shared" si="6"/>
+        <v>3.9744262645914397</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="6"/>
+        <v>3.9966236869565219</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="6"/>
+        <v>3.9625174439024393</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="6"/>
+        <v>3.9856597268292684</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="6"/>
+        <v>3.9653104780487802</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="6"/>
+        <v>3.9517443121951215</v>
       </c>
     </row>
     <row r="49" spans="1:15">
-      <c r="A49" t="s">
-        <v>65</v>
-      </c>
-      <c r="N49">
-        <f>N48*0.995</f>
-        <v>1223.8499999999999</v>
-      </c>
-      <c r="O49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15">
-      <c r="N50">
-        <f>N49*0.995</f>
-        <v>1217.7307499999999</v>
-      </c>
-      <c r="O50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15">
-      <c r="A51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B51">
-        <v>2.5</v>
-      </c>
-      <c r="N51">
-        <f>N50*0.995</f>
-        <v>1211.6420962499999</v>
-      </c>
-      <c r="O51" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15">
-      <c r="A52" t="s">
-        <v>63</v>
-      </c>
-      <c r="B52">
-        <v>137.5</v>
-      </c>
-      <c r="N52">
-        <f>N51*0.995</f>
-        <v>1205.58388576875</v>
-      </c>
-      <c r="O52" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15">
-      <c r="A53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53">
-        <v>7.1014699999999999</v>
-      </c>
-      <c r="N53">
-        <v>1100</v>
-      </c>
-      <c r="O53" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15">
-      <c r="A54" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54">
-        <v>12.23232</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15">
-      <c r="A55" t="s">
-        <v>68</v>
-      </c>
-      <c r="B55">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15">
-      <c r="A56" t="s">
-        <v>69</v>
-      </c>
-      <c r="B56">
-        <f>B52-B51</f>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" t="s">
-        <v>70</v>
-      </c>
-      <c r="B57">
-        <f>B56/B55</f>
-        <v>0.1125</v>
+      <c r="G49" t="s">
+        <v>54</v>
+      </c>
+      <c r="K49" t="s">
+        <v>58</v>
+      </c>
+      <c r="L49" t="s">
+        <v>58</v>
+      </c>
+      <c r="M49" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58">
-        <f>B57*60</f>
-        <v>6.75</v>
+        <v>64</v>
+      </c>
+      <c r="N58">
+        <v>1230</v>
+      </c>
+      <c r="O58" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" t="s">
+        <v>65</v>
+      </c>
+      <c r="N59">
+        <f>N58*0.995</f>
+        <v>1223.8499999999999</v>
+      </c>
+      <c r="O59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="N60">
+        <f>N59*0.995</f>
+        <v>1217.7307499999999</v>
+      </c>
+      <c r="O60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61">
+        <v>2.5</v>
+      </c>
+      <c r="N61">
+        <f>N60*0.995</f>
+        <v>1211.6420962499999</v>
+      </c>
+      <c r="O61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62">
+        <v>137.5</v>
+      </c>
+      <c r="N62">
+        <f>N61*0.995</f>
+        <v>1205.58388576875</v>
+      </c>
+      <c r="O62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63">
+        <v>7.1014699999999999</v>
+      </c>
+      <c r="N63">
+        <v>1100</v>
+      </c>
+      <c r="O63" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64">
+        <v>12.23232</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66">
+        <f>B62-B61</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67">
+        <f>B66/B65</f>
+        <v>0.1125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68">
+        <f>B67*60</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
         <v>72</v>
       </c>
-      <c r="B59">
-        <f>B54-B53</f>
+      <c r="B69">
+        <f>B64-B63</f>
         <v>5.1308499999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
-      <c r="A60" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
         <v>73</v>
       </c>
-      <c r="B60">
-        <f>B59/B57</f>
+      <c r="B70">
+        <f>B69/B67</f>
         <v>45.60755555555555</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved dimensions to dependencencies
</commit_message>
<xml_diff>
--- a/logs/calibration analysis.xlsx
+++ b/logs/calibration analysis.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="310" windowWidth="15060" windowHeight="7060" activeTab="2"/>
+    <workbookView xWindow="560" yWindow="310" windowWidth="15060" windowHeight="7060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2017-10-05" sheetId="1" r:id="rId1"/>
     <sheet name="2017-10-07" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="103">
   <si>
     <t>Nominal</t>
   </si>
@@ -253,14 +254,88 @@
   </si>
   <si>
     <t>On RepRapPro site</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>Length (mm)</t>
+  </si>
+  <si>
+    <t>Diam</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Est volume mm3</t>
+  </si>
+  <si>
+    <t>Est volume cm3</t>
+  </si>
+  <si>
+    <t>Filament length for cube according to cura</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>cm3</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>g/cm3</t>
+  </si>
+  <si>
+    <t>Cube 1</t>
+  </si>
+  <si>
+    <t>Cube 2</t>
+  </si>
+  <si>
+    <t>Cube 3</t>
+  </si>
+  <si>
+    <t>Cube 4</t>
+  </si>
+  <si>
+    <t>Extrusion</t>
+  </si>
+  <si>
+    <t>steps/mm</t>
+  </si>
+  <si>
+    <t>required esteps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -326,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -340,6 +415,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +524,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.11951224846894153"/>
+                  <c:x val="0.11951224846894161"/>
                   <c:y val="0.26999489647127445"/>
                 </c:manualLayout>
               </c:layout>
@@ -491,23 +568,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="70984832"/>
-        <c:axId val="70986368"/>
+        <c:axId val="86848256"/>
+        <c:axId val="86849792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70984832"/>
+        <c:axId val="86848256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70986368"/>
+        <c:crossAx val="86849792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70986368"/>
+        <c:axId val="86849792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +592,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70984832"/>
+        <c:crossAx val="86848256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -527,7 +604,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -660,30 +737,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="71011328"/>
-        <c:axId val="71037696"/>
+        <c:axId val="86870656"/>
+        <c:axId val="86897024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71011328"/>
+        <c:axId val="86870656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71037696"/>
+        <c:crossAx val="86897024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71037696"/>
+        <c:axId val="86897024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71011328"/>
+        <c:crossAx val="86870656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -695,7 +772,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -736,7 +813,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18876507790249644"/>
+                  <c:x val="-0.18876507790249658"/>
                   <c:y val="1.0198625702291192E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -828,30 +905,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87528576"/>
-        <c:axId val="87530112"/>
+        <c:axId val="88965888"/>
+        <c:axId val="88967424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87528576"/>
+        <c:axId val="88965888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87530112"/>
+        <c:crossAx val="88967424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87530112"/>
+        <c:axId val="88967424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87528576"/>
+        <c:crossAx val="88965888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -863,7 +940,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -920,7 +997,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18876507790249653"/>
+                  <c:x val="-0.18876507790249669"/>
                   <c:y val="1.0198625702291192E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -1012,30 +1089,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95890432"/>
-        <c:axId val="95912704"/>
+        <c:axId val="89078400"/>
+        <c:axId val="89088384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95890432"/>
+        <c:axId val="89078400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95912704"/>
+        <c:crossAx val="89088384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95912704"/>
+        <c:axId val="89088384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95890432"/>
+        <c:crossAx val="89078400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1047,7 +1124,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1088,8 +1165,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.7630675154967344E-3"/>
-                  <c:y val="-5.7164936611040391E-3"/>
+                  <c:x val="1.7630675154967357E-3"/>
+                  <c:y val="-5.7164936611040443E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1186,30 +1263,30 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95933568"/>
-        <c:axId val="95935104"/>
+        <c:axId val="89109248"/>
+        <c:axId val="89110784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95933568"/>
+        <c:axId val="89109248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95935104"/>
+        <c:crossAx val="89110784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95935104"/>
+        <c:axId val="89110784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95933568"/>
+        <c:crossAx val="89109248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1221,7 +1298,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2348,10 +2425,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S70"/>
+  <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2406,981 +2483,1138 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>5.35</v>
+        <v>7.55</v>
       </c>
       <c r="G5" s="6">
         <f>B5*C5*(D5/E5)/(F5*PI())</f>
-        <v>917.33826162737307</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
-      <c r="A12" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
-      <c r="A13" s="3"/>
+        <v>633.05236661310187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>630</v>
+      </c>
+      <c r="C9">
+        <v>620</v>
+      </c>
+      <c r="D9">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>120</v>
+      </c>
+      <c r="C12">
+        <v>119.9</v>
+      </c>
+      <c r="D12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>18.41</v>
+      </c>
+      <c r="C13">
+        <v>19.03</v>
+      </c>
+      <c r="D13">
+        <v>23.5</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:C14" si="0">B12-B13</f>
+        <v>101.59</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>100.87</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14" si="1">D12-D13</f>
+        <v>96.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="5">
+        <f t="shared" ref="B15:C15" si="2">B11/B14</f>
+        <v>0.9843488532335859</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="2"/>
+        <v>0.99137503717656383</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" ref="D15" si="3">D11/D14</f>
+        <v>1.0362694300518134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:C16" si="4">B9*B15</f>
+        <v>620.13977753715915</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="4"/>
+        <v>614.65252304946955</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16" si="5">D9*D15</f>
+        <v>642.48704663212425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17">
+        <f>4907.76/B16</f>
+        <v>7.913957752380953</v>
+      </c>
+      <c r="C17">
+        <f>4907.76/C16</f>
+        <v>7.9846088903225816</v>
+      </c>
+      <c r="D17">
+        <f>4907.76/D16</f>
+        <v>7.6386909677419368</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1">
+      <c r="A23" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="43.5">
-      <c r="B17" s="4" t="s">
+    <row r="28" spans="1:7" ht="43.5">
+      <c r="B28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B18">
+      <c r="B29">
         <v>200</v>
       </c>
-      <c r="C18">
+      <c r="C29">
         <v>16</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4">
         <v>920</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19">
-        <v>200</v>
-      </c>
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19">
-        <v>53</v>
-      </c>
-      <c r="E19">
-        <v>11</v>
-      </c>
-      <c r="F19">
-        <v>5.35</v>
-      </c>
-      <c r="G19" s="6">
-        <f>B19*C19*(D19/E19)/(F19*PI())</f>
-        <v>917.33826162737307</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20">
-        <v>200</v>
-      </c>
-      <c r="C20">
-        <v>16</v>
-      </c>
-      <c r="D20">
-        <v>53</v>
-      </c>
-      <c r="E20">
-        <v>9</v>
-      </c>
-      <c r="F20">
-        <v>5.35</v>
-      </c>
-      <c r="G20" s="6">
-        <f>B20*C20*(D20/E20)/(F20*PI())</f>
-        <v>1121.1912086556781</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21">
-        <v>200</v>
-      </c>
-      <c r="C21">
-        <v>16</v>
-      </c>
-      <c r="D21">
-        <v>53</v>
-      </c>
-      <c r="E21">
-        <v>11</v>
-      </c>
-      <c r="F21" s="6">
-        <f>((B21*C21)*(D21/E21))/G21/PI()</f>
-        <v>4.6911774205542951</v>
-      </c>
-      <c r="G21">
-        <v>1046.1679999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22">
-        <v>200</v>
-      </c>
-      <c r="C22">
-        <v>16</v>
-      </c>
-      <c r="D22">
-        <v>53</v>
-      </c>
-      <c r="E22">
-        <v>11</v>
-      </c>
-      <c r="F22" s="6">
-        <f>((B22*C22)*(D22/E22))/G22/PI()</f>
-        <v>5.3345214127243974</v>
-      </c>
-      <c r="G22">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="F23">
-        <f>((B22*C22)*(D22/E22))/PI()</f>
-        <v>4907.7596997064456</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>200</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>53</v>
+      </c>
+      <c r="E30">
+        <v>11</v>
+      </c>
+      <c r="F30">
+        <v>5.35</v>
+      </c>
+      <c r="G30" s="6">
+        <f>B30*C30*(D30/E30)/(F30*PI())</f>
+        <v>917.33826162737307</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>200</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <v>53</v>
+      </c>
+      <c r="E31">
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <v>5.35</v>
+      </c>
+      <c r="G31" s="6">
+        <f>B31*C31*(D31/E31)/(F31*PI())</f>
+        <v>1121.1912086556781</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32">
+        <v>200</v>
+      </c>
+      <c r="C32">
+        <v>16</v>
+      </c>
+      <c r="D32">
+        <v>53</v>
+      </c>
+      <c r="E32">
+        <v>11</v>
+      </c>
+      <c r="F32" s="6">
+        <f>((B32*C32)*(D32/E32))/G32/PI()</f>
+        <v>4.6911774205542951</v>
+      </c>
+      <c r="G32">
+        <v>1046.1679999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33">
+        <v>200</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>53</v>
+      </c>
+      <c r="E33">
+        <v>11</v>
+      </c>
+      <c r="F33" s="6">
+        <f>((B33*C33)*(D33/E33))/G33/PI()</f>
+        <v>5.3345214127243974</v>
+      </c>
+      <c r="G33">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="F34">
+        <f>((B33*C33)*(D33/E33))/PI()</f>
+        <v>4907.7596997064456</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
-      <c r="A33" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
-      <c r="A34" t="s">
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
-      <c r="A35" t="s">
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
-      <c r="A38" t="s">
+    <row r="49" spans="1:19">
+      <c r="A49" t="s">
         <v>42</v>
       </c>
-      <c r="B38">
+      <c r="B49">
         <v>1</v>
       </c>
-      <c r="C38">
+      <c r="C49">
         <v>2</v>
       </c>
-      <c r="D38">
+      <c r="D49">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
-      <c r="A39" t="s">
+    <row r="50" spans="1:19">
+      <c r="A50" t="s">
         <v>51</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B50" t="s">
         <v>52</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C50" t="s">
         <v>53</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K50" t="s">
         <v>57</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L50" t="s">
         <v>59</v>
       </c>
-      <c r="R39" s="7" t="s">
+      <c r="R50" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S39" s="7" t="s">
+      <c r="S50" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
-      <c r="A40" t="s">
+    <row r="51" spans="1:19">
+      <c r="A51" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
+      <c r="B51">
         <v>920</v>
       </c>
-      <c r="C40">
+      <c r="C51">
         <v>920</v>
       </c>
-      <c r="D40">
+      <c r="D51">
         <v>920</v>
       </c>
-      <c r="E40">
+      <c r="E51">
         <v>920</v>
       </c>
-      <c r="F40">
+      <c r="F51">
         <v>1028</v>
       </c>
-      <c r="G40">
+      <c r="G51">
         <v>1028</v>
       </c>
-      <c r="H40">
+      <c r="H51">
         <v>1028</v>
       </c>
-      <c r="I40">
+      <c r="I51">
         <v>1028</v>
       </c>
-      <c r="J40">
+      <c r="J51">
         <v>1028</v>
       </c>
-      <c r="K40">
+      <c r="K51">
         <v>1028</v>
       </c>
-      <c r="L40">
+      <c r="L51">
         <v>1028</v>
       </c>
-      <c r="M40">
+      <c r="M51">
         <v>1028</v>
       </c>
-      <c r="N40">
+      <c r="N51">
         <v>1028</v>
       </c>
-      <c r="O40">
+      <c r="O51">
         <v>920</v>
       </c>
-      <c r="P40">
+      <c r="P51">
         <v>1230</v>
       </c>
-      <c r="Q40">
+      <c r="Q51">
         <v>1230</v>
       </c>
-      <c r="R40">
+      <c r="R51">
         <v>1230</v>
       </c>
-      <c r="S40">
+      <c r="S51">
         <v>1230</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
-      <c r="A41" t="s">
+    <row r="52" spans="1:19">
+      <c r="A52" t="s">
         <v>55</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B52" t="s">
         <v>56</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C52" t="s">
         <v>56</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D52" t="s">
         <v>56</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E52" t="s">
         <v>56</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F52" t="s">
         <v>56</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G52" t="s">
         <v>56</v>
       </c>
-      <c r="H41">
+      <c r="H52">
         <v>10</v>
       </c>
-      <c r="I41">
+      <c r="I52">
         <v>300</v>
       </c>
-      <c r="J41">
+      <c r="J52">
         <v>600</v>
       </c>
-      <c r="K41">
+      <c r="K52">
         <v>600</v>
       </c>
-      <c r="L41">
+      <c r="L52">
         <v>600</v>
       </c>
-      <c r="M41">
+      <c r="M52">
         <v>300</v>
       </c>
-      <c r="N41">
+      <c r="N52">
         <v>100</v>
       </c>
-      <c r="O41">
+      <c r="O52">
         <v>100</v>
       </c>
-      <c r="P41">
+      <c r="P52">
         <v>100</v>
       </c>
-      <c r="Q41">
+      <c r="Q52">
         <v>50</v>
       </c>
-      <c r="R41">
+      <c r="R52">
         <v>100</v>
       </c>
-      <c r="S41">
+      <c r="S52">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
-      <c r="A42" t="s">
+    <row r="53" spans="1:19">
+      <c r="A53" t="s">
         <v>43</v>
       </c>
-      <c r="B42">
+      <c r="B53">
         <v>100</v>
       </c>
-      <c r="C42">
+      <c r="C53">
         <v>100</v>
       </c>
-      <c r="D42">
+      <c r="D53">
         <v>100</v>
       </c>
-      <c r="E42">
+      <c r="E53">
         <v>100</v>
       </c>
-      <c r="F42">
+      <c r="F53">
         <v>100</v>
       </c>
-      <c r="G42">
+      <c r="G53">
         <v>100</v>
       </c>
-      <c r="H42">
+      <c r="H53">
         <v>100</v>
       </c>
-      <c r="I42">
+      <c r="I53">
         <v>100</v>
       </c>
-      <c r="J42">
+      <c r="J53">
         <v>100</v>
       </c>
-      <c r="K42">
+      <c r="K53">
         <v>100</v>
       </c>
-      <c r="L42">
+      <c r="L53">
         <v>100</v>
       </c>
-      <c r="M42">
+      <c r="M53">
         <v>100</v>
       </c>
-      <c r="N42">
+      <c r="N53">
         <v>100</v>
       </c>
-      <c r="O42">
+      <c r="O53">
         <v>100</v>
       </c>
-      <c r="P42">
+      <c r="P53">
         <v>100</v>
       </c>
-      <c r="Q42">
+      <c r="Q53">
         <v>100</v>
       </c>
-      <c r="R42">
+      <c r="R53">
         <v>100</v>
       </c>
-      <c r="S42">
+      <c r="S53">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
-      <c r="A43" t="s">
+    <row r="54" spans="1:19">
+      <c r="A54" t="s">
         <v>44</v>
       </c>
-      <c r="B43">
+      <c r="B54">
         <v>124.9</v>
       </c>
-      <c r="C43">
+      <c r="C54">
         <v>119.98</v>
       </c>
-      <c r="D43">
+      <c r="D54">
         <v>120.22</v>
       </c>
-      <c r="E43">
+      <c r="E54">
         <v>120.37</v>
       </c>
-      <c r="F43">
+      <c r="F54">
         <v>120.37</v>
       </c>
-      <c r="G43">
+      <c r="G54">
         <v>120.45</v>
       </c>
-      <c r="H43">
+      <c r="H54">
         <v>120.54</v>
       </c>
-      <c r="I43">
+      <c r="I54">
         <v>120.64</v>
       </c>
-      <c r="J43">
+      <c r="J54">
         <v>120.57</v>
       </c>
-      <c r="K43">
+      <c r="K54">
         <v>120.52</v>
       </c>
-      <c r="L43">
+      <c r="L54">
         <v>120</v>
       </c>
-      <c r="M43">
+      <c r="M54">
         <v>120</v>
       </c>
-      <c r="N43">
+      <c r="N54">
         <v>120.27</v>
       </c>
-      <c r="O43">
+      <c r="O54">
         <v>120.22</v>
       </c>
-      <c r="P43">
+      <c r="P54">
         <v>120.43</v>
       </c>
-      <c r="Q43">
+      <c r="Q54">
         <v>120.37</v>
       </c>
-      <c r="R43">
+      <c r="R54">
         <v>119.64</v>
       </c>
-      <c r="S43">
+      <c r="S54">
         <v>120.02</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
-      <c r="A44" t="s">
+    <row r="55" spans="1:19">
+      <c r="A55" t="s">
         <v>45</v>
       </c>
-      <c r="B44">
+      <c r="B55">
         <v>36.96</v>
       </c>
-      <c r="C44">
+      <c r="C55">
         <v>18.95</v>
       </c>
-      <c r="D44">
+      <c r="D55">
         <v>29.3</v>
       </c>
-      <c r="E44">
+      <c r="E55">
         <v>30.86</v>
       </c>
-      <c r="F44">
+      <c r="F55">
         <v>33.799999999999997</v>
       </c>
-      <c r="G44">
+      <c r="G55">
         <v>36.68</v>
       </c>
-      <c r="H44">
+      <c r="H55">
         <v>37.24</v>
       </c>
-      <c r="I44">
+      <c r="I55">
         <v>55.09</v>
       </c>
-      <c r="J44">
+      <c r="J55">
         <v>25.27</v>
       </c>
-      <c r="K44">
+      <c r="K55">
         <v>89.04</v>
       </c>
-      <c r="L44">
+      <c r="L55">
         <v>87.37</v>
       </c>
-      <c r="N44">
+      <c r="N55">
         <v>37.020000000000003</v>
       </c>
-      <c r="O44">
+      <c r="O55">
         <v>45.3</v>
       </c>
-      <c r="P44">
+      <c r="P55">
         <v>21.12</v>
       </c>
-      <c r="Q44">
+      <c r="Q55">
         <v>20.48</v>
       </c>
-      <c r="R44">
+      <c r="R55">
         <v>20.260000000000002</v>
       </c>
-      <c r="S44">
+      <c r="S55">
         <v>20.98</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
-      <c r="A45" t="s">
+    <row r="56" spans="1:19">
+      <c r="A56" t="s">
         <v>46</v>
       </c>
-      <c r="B45">
-        <f t="shared" ref="B45:G45" si="0">B43-B44</f>
+      <c r="B56">
+        <f t="shared" ref="B56:G56" si="6">B54-B55</f>
         <v>87.94</v>
       </c>
-      <c r="C45">
-        <f t="shared" si="0"/>
+      <c r="C56">
+        <f t="shared" si="6"/>
         <v>101.03</v>
       </c>
-      <c r="D45">
-        <f t="shared" si="0"/>
+      <c r="D56">
+        <f t="shared" si="6"/>
         <v>90.92</v>
       </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
+      <c r="E56">
+        <f t="shared" si="6"/>
         <v>89.51</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="0"/>
+      <c r="F56">
+        <f t="shared" si="6"/>
         <v>86.570000000000007</v>
       </c>
-      <c r="G45">
-        <f t="shared" si="0"/>
+      <c r="G56">
+        <f t="shared" si="6"/>
         <v>83.77000000000001</v>
       </c>
-      <c r="H45">
-        <f t="shared" ref="H45:S45" si="1">H43-H44</f>
+      <c r="H56">
+        <f t="shared" ref="H56:S56" si="7">H54-H55</f>
         <v>83.300000000000011</v>
       </c>
-      <c r="I45">
-        <f t="shared" si="1"/>
+      <c r="I56">
+        <f t="shared" si="7"/>
         <v>65.55</v>
       </c>
-      <c r="J45">
-        <f t="shared" si="1"/>
+      <c r="J56">
+        <f t="shared" si="7"/>
         <v>95.3</v>
       </c>
-      <c r="K45">
-        <f t="shared" si="1"/>
+      <c r="K56">
+        <f t="shared" si="7"/>
         <v>31.47999999999999</v>
       </c>
-      <c r="L45">
-        <f t="shared" si="1"/>
+      <c r="L56">
+        <f t="shared" si="7"/>
         <v>32.629999999999995</v>
       </c>
-      <c r="N45">
-        <f t="shared" si="1"/>
+      <c r="N56">
+        <f t="shared" si="7"/>
         <v>83.25</v>
       </c>
-      <c r="O45">
-        <f t="shared" si="1"/>
+      <c r="O56">
+        <f t="shared" si="7"/>
         <v>74.92</v>
       </c>
-      <c r="P45">
-        <f t="shared" si="1"/>
+      <c r="P56">
+        <f t="shared" si="7"/>
         <v>99.31</v>
       </c>
-      <c r="Q45">
-        <f t="shared" si="1"/>
+      <c r="Q56">
+        <f t="shared" si="7"/>
         <v>99.89</v>
       </c>
-      <c r="R45">
-        <f t="shared" si="1"/>
+      <c r="R56">
+        <f t="shared" si="7"/>
         <v>99.38</v>
       </c>
-      <c r="S45">
-        <f t="shared" si="1"/>
+      <c r="S56">
+        <f t="shared" si="7"/>
         <v>99.039999999999992</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
-      <c r="A46" t="s">
+    <row r="57" spans="1:19">
+      <c r="A57" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="5">
-        <f t="shared" ref="B46:G46" si="2">B42/B45</f>
+      <c r="B57" s="5">
+        <f t="shared" ref="B57:G57" si="8">B53/B56</f>
         <v>1.1371389583807141</v>
       </c>
-      <c r="C46" s="5">
-        <f t="shared" si="2"/>
+      <c r="C57" s="5">
+        <f t="shared" si="8"/>
         <v>0.98980500841334251</v>
       </c>
-      <c r="D46" s="5">
-        <f t="shared" si="2"/>
+      <c r="D57" s="5">
+        <f t="shared" si="8"/>
         <v>1.0998680158380993</v>
       </c>
-      <c r="E46" s="5">
-        <f t="shared" si="2"/>
+      <c r="E57" s="5">
+        <f t="shared" si="8"/>
         <v>1.1171936096525528</v>
       </c>
-      <c r="F46" s="5">
-        <f t="shared" si="2"/>
+      <c r="F57" s="5">
+        <f t="shared" si="8"/>
         <v>1.1551345731777751</v>
       </c>
-      <c r="G46" s="5">
-        <f t="shared" si="2"/>
+      <c r="G57" s="5">
+        <f t="shared" si="8"/>
         <v>1.1937447773665988</v>
       </c>
-      <c r="H46" s="5">
-        <f t="shared" ref="H46:S46" si="3">H42/H45</f>
+      <c r="H57" s="5">
+        <f t="shared" ref="H57:S57" si="9">H53/H56</f>
         <v>1.2004801920768307</v>
       </c>
-      <c r="I46" s="5">
-        <f t="shared" si="3"/>
+      <c r="I57" s="5">
+        <f t="shared" si="9"/>
         <v>1.5255530129672006</v>
       </c>
-      <c r="J46" s="5">
-        <f t="shared" si="3"/>
+      <c r="J57" s="5">
+        <f t="shared" si="9"/>
         <v>1.0493179433368311</v>
       </c>
-      <c r="K46" s="5">
-        <f t="shared" si="3"/>
+      <c r="K57" s="5">
+        <f t="shared" si="9"/>
         <v>3.176620076238883</v>
       </c>
-      <c r="L46" s="5">
-        <f t="shared" si="3"/>
+      <c r="L57" s="5">
+        <f t="shared" si="9"/>
         <v>3.064664419246093</v>
       </c>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5">
-        <f t="shared" si="3"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5">
+        <f t="shared" si="9"/>
         <v>1.2012012012012012</v>
       </c>
-      <c r="O46" s="5">
-        <f t="shared" si="3"/>
+      <c r="O57" s="5">
+        <f t="shared" si="9"/>
         <v>1.3347570742124932</v>
       </c>
-      <c r="P46" s="5">
-        <f t="shared" si="3"/>
+      <c r="P57" s="5">
+        <f t="shared" si="9"/>
         <v>1.006947940791461</v>
       </c>
-      <c r="Q46" s="5">
-        <f t="shared" si="3"/>
+      <c r="Q57" s="5">
+        <f t="shared" si="9"/>
         <v>1.0011012113324658</v>
       </c>
-      <c r="R46" s="5">
-        <f t="shared" si="3"/>
+      <c r="R57" s="5">
+        <f t="shared" si="9"/>
         <v>1.0062386798148522</v>
       </c>
-      <c r="S46" s="5">
-        <f t="shared" si="3"/>
+      <c r="S57" s="5">
+        <f t="shared" si="9"/>
         <v>1.0096930533117934</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
-      <c r="A47" t="s">
+    <row r="58" spans="1:19">
+      <c r="A58" t="s">
         <v>48</v>
       </c>
-      <c r="B47">
-        <f t="shared" ref="B47:G47" si="4">B40*B46</f>
+      <c r="B58">
+        <f t="shared" ref="B58:G58" si="10">B51*B57</f>
         <v>1046.1678417102569</v>
       </c>
-      <c r="C47">
-        <f t="shared" si="4"/>
+      <c r="C58">
+        <f t="shared" si="10"/>
         <v>910.62060774027509</v>
       </c>
-      <c r="D47">
-        <f t="shared" si="4"/>
+      <c r="D58">
+        <f t="shared" si="10"/>
         <v>1011.8785745710514</v>
       </c>
-      <c r="E47">
-        <f t="shared" si="4"/>
+      <c r="E58">
+        <f t="shared" si="10"/>
         <v>1027.8181208803485</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="4"/>
+      <c r="F58">
+        <f t="shared" si="10"/>
         <v>1187.4783412267527</v>
       </c>
-      <c r="G47">
-        <f t="shared" si="4"/>
+      <c r="G58">
+        <f t="shared" si="10"/>
         <v>1227.1696311328635</v>
       </c>
-      <c r="H47">
-        <f t="shared" ref="H47:S47" si="5">H40*H46</f>
+      <c r="H58">
+        <f t="shared" ref="H58:S58" si="11">H51*H57</f>
         <v>1234.0936374549819</v>
       </c>
-      <c r="I47">
-        <f t="shared" si="5"/>
+      <c r="I58">
+        <f t="shared" si="11"/>
         <v>1568.2684973302821</v>
       </c>
-      <c r="J47">
-        <f t="shared" si="5"/>
+      <c r="J58">
+        <f t="shared" si="11"/>
         <v>1078.6988457502625</v>
       </c>
-      <c r="K47">
-        <f t="shared" si="5"/>
+      <c r="K58">
+        <f t="shared" si="11"/>
         <v>3265.5654383735719</v>
       </c>
-      <c r="L47">
-        <f t="shared" si="5"/>
+      <c r="L58">
+        <f t="shared" si="11"/>
         <v>3150.4750229849838</v>
       </c>
-      <c r="N47">
-        <f t="shared" si="5"/>
+      <c r="N58">
+        <f t="shared" si="11"/>
         <v>1234.834834834835</v>
       </c>
-      <c r="O47">
-        <f t="shared" si="5"/>
+      <c r="O58">
+        <f t="shared" si="11"/>
         <v>1227.9765082754939</v>
       </c>
-      <c r="P47">
-        <f t="shared" si="5"/>
+      <c r="P58">
+        <f t="shared" si="11"/>
         <v>1238.545967173497</v>
       </c>
-      <c r="Q47">
-        <f t="shared" si="5"/>
+      <c r="Q58">
+        <f t="shared" si="11"/>
         <v>1231.3544899389328</v>
       </c>
-      <c r="R47">
-        <f t="shared" si="5"/>
+      <c r="R58">
+        <f t="shared" si="11"/>
         <v>1237.6735761722682</v>
       </c>
-      <c r="S47">
-        <f t="shared" si="5"/>
+      <c r="S58">
+        <f t="shared" si="11"/>
         <v>1241.9224555735059</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
-      <c r="A48" t="s">
+    <row r="59" spans="1:19">
+      <c r="A59" t="s">
         <v>49</v>
       </c>
-      <c r="B48">
-        <f>4907.76/B47</f>
+      <c r="B59">
+        <f>4907.76/B58</f>
         <v>4.6911784173913054</v>
       </c>
-      <c r="C48">
-        <f t="shared" ref="C48:S48" si="6">4907.76/C47</f>
+      <c r="C59">
+        <f t="shared" ref="C59:S59" si="12">4907.76/C58</f>
         <v>5.3894673130434789</v>
       </c>
-      <c r="D48">
-        <f t="shared" si="6"/>
+      <c r="D59">
+        <f t="shared" si="12"/>
         <v>4.8501471652173915</v>
       </c>
-      <c r="E48">
-        <f t="shared" si="6"/>
+      <c r="E59">
+        <f t="shared" si="12"/>
         <v>4.7749304086956528</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="6"/>
+      <c r="F59">
+        <f t="shared" si="12"/>
         <v>4.132925906614787</v>
       </c>
-      <c r="G48">
-        <f t="shared" si="6"/>
+      <c r="G59">
+        <f t="shared" si="12"/>
         <v>3.9992515097276273</v>
       </c>
-      <c r="H48">
-        <f t="shared" si="6"/>
+      <c r="H59">
+        <f t="shared" si="12"/>
         <v>3.9768133073929963</v>
       </c>
-      <c r="I48">
-        <f t="shared" si="6"/>
+      <c r="I59">
+        <f t="shared" si="12"/>
         <v>3.1294131128404672</v>
       </c>
-      <c r="J48">
-        <f t="shared" si="6"/>
+      <c r="J59">
+        <f t="shared" si="12"/>
         <v>4.5497035797665362</v>
       </c>
-      <c r="K48">
-        <f t="shared" si="6"/>
+      <c r="K59">
+        <f t="shared" si="12"/>
         <v>1.5028821478599217</v>
       </c>
-      <c r="L48">
-        <f t="shared" si="6"/>
+      <c r="L59">
+        <f t="shared" si="12"/>
         <v>1.5577841322957195</v>
       </c>
-      <c r="N48">
-        <f t="shared" si="6"/>
+      <c r="N59">
+        <f t="shared" si="12"/>
         <v>3.9744262645914397</v>
       </c>
-      <c r="O48">
-        <f t="shared" si="6"/>
+      <c r="O59">
+        <f t="shared" si="12"/>
         <v>3.9966236869565219</v>
       </c>
-      <c r="P48">
-        <f t="shared" si="6"/>
+      <c r="P59">
+        <f t="shared" si="12"/>
         <v>3.9625174439024393</v>
       </c>
-      <c r="Q48">
-        <f t="shared" si="6"/>
+      <c r="Q59">
+        <f t="shared" si="12"/>
         <v>3.9856597268292684</v>
       </c>
-      <c r="R48">
-        <f t="shared" si="6"/>
+      <c r="R59">
+        <f t="shared" si="12"/>
         <v>3.9653104780487802</v>
       </c>
-      <c r="S48">
-        <f t="shared" si="6"/>
+      <c r="S59">
+        <f t="shared" si="12"/>
         <v>3.9517443121951215</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
-      <c r="G49" t="s">
+    <row r="60" spans="1:19">
+      <c r="G60" t="s">
         <v>54</v>
       </c>
-      <c r="K49" t="s">
+      <c r="K60" t="s">
         <v>58</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L60" t="s">
         <v>58</v>
       </c>
-      <c r="M49" t="s">
+      <c r="M60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
-      <c r="A58" t="s">
+    <row r="69" spans="1:15">
+      <c r="A69" t="s">
         <v>64</v>
       </c>
-      <c r="N58">
+      <c r="N69">
         <v>1230</v>
       </c>
-      <c r="O58" t="s">
+      <c r="O69" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
-      <c r="A59" t="s">
+    <row r="70" spans="1:15">
+      <c r="A70" t="s">
         <v>65</v>
       </c>
-      <c r="N59">
-        <f>N58*0.995</f>
+      <c r="N70">
+        <f>N69*0.995</f>
         <v>1223.8499999999999</v>
       </c>
-      <c r="O59" t="s">
+      <c r="O70" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
-      <c r="N60">
-        <f>N59*0.995</f>
+    <row r="71" spans="1:15">
+      <c r="N71">
+        <f>N70*0.995</f>
         <v>1217.7307499999999</v>
       </c>
-      <c r="O60" t="s">
+      <c r="O71" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
-      <c r="A61" t="s">
+    <row r="72" spans="1:15">
+      <c r="A72" t="s">
         <v>62</v>
       </c>
-      <c r="B61">
+      <c r="B72">
         <v>2.5</v>
       </c>
-      <c r="N61">
-        <f>N60*0.995</f>
+      <c r="N72">
+        <f>N71*0.995</f>
         <v>1211.6420962499999</v>
       </c>
-      <c r="O61" t="s">
+      <c r="O72" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
-      <c r="A62" t="s">
+    <row r="73" spans="1:15">
+      <c r="A73" t="s">
         <v>63</v>
       </c>
-      <c r="B62">
+      <c r="B73">
         <v>137.5</v>
       </c>
-      <c r="N62">
-        <f>N61*0.995</f>
+      <c r="N73">
+        <f>N72*0.995</f>
         <v>1205.58388576875</v>
       </c>
-      <c r="O62" t="s">
+      <c r="O73" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
-      <c r="A63" t="s">
+    <row r="74" spans="1:15">
+      <c r="A74" t="s">
         <v>66</v>
       </c>
-      <c r="B63">
+      <c r="B74">
         <v>7.1014699999999999</v>
       </c>
-      <c r="N63">
+      <c r="N74">
         <v>1100</v>
       </c>
-      <c r="O63" t="s">
+      <c r="O74" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
-      <c r="A64" t="s">
+    <row r="75" spans="1:15">
+      <c r="A75" t="s">
         <v>67</v>
       </c>
-      <c r="B64">
+      <c r="B75">
         <v>12.23232</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
+    <row r="76" spans="1:15">
+      <c r="A76" t="s">
         <v>68</v>
       </c>
-      <c r="B65">
+      <c r="B76">
         <v>1200</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
+    <row r="77" spans="1:15">
+      <c r="A77" t="s">
         <v>69</v>
       </c>
-      <c r="B66">
-        <f>B62-B61</f>
+      <c r="B77">
+        <f>B73-B72</f>
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
+    <row r="78" spans="1:15">
+      <c r="A78" t="s">
         <v>70</v>
       </c>
-      <c r="B67">
-        <f>B66/B65</f>
+      <c r="B78">
+        <f>B77/B76</f>
         <v>0.1125</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
+    <row r="79" spans="1:15">
+      <c r="A79" t="s">
         <v>71</v>
       </c>
-      <c r="B68">
-        <f>B67*60</f>
+      <c r="B79">
+        <f>B78*60</f>
         <v>6.75</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
+    <row r="80" spans="1:15">
+      <c r="A80" t="s">
         <v>72</v>
       </c>
-      <c r="B69">
-        <f>B64-B63</f>
+      <c r="B80">
+        <f>B75-B74</f>
         <v>5.1308499999999997</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
         <v>73</v>
       </c>
-      <c r="B70">
-        <f>B69/B67</f>
+      <c r="B81">
+        <f>B80/B78</f>
         <v>45.60755555555555</v>
       </c>
     </row>
@@ -3388,4 +3622,260 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="5" width="20.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2">
+        <v>1.75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f>10.5*10</f>
+        <v>105</v>
+      </c>
+      <c r="C6">
+        <v>0.32</v>
+      </c>
+      <c r="D6">
+        <f>PI()*($B$2/2)^2*B6</f>
+        <v>252.55459691749195</v>
+      </c>
+      <c r="E6" s="10">
+        <f>B6/10*($B$2/20)^2*PI()</f>
+        <v>0.25255459691749194</v>
+      </c>
+      <c r="F6">
+        <f>C6/E6</f>
+        <v>1.2670527636625917</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>99</v>
+      </c>
+      <c r="C7">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D7">
+        <f>PI()*($B$2/2)^2*B7</f>
+        <v>238.12290566506383</v>
+      </c>
+      <c r="E7" s="10">
+        <f>B7/10*($B$2/20)^2*PI()</f>
+        <v>0.23812290566506386</v>
+      </c>
+      <c r="F7">
+        <f>C7/E7</f>
+        <v>1.2178584802249339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>0.3</v>
+      </c>
+      <c r="D8">
+        <f>PI()*($B$2/2)^2*B8</f>
+        <v>240.52818754046851</v>
+      </c>
+      <c r="E8" s="10">
+        <f>B8/10*($B$2/20)^2*PI()</f>
+        <v>0.24052818754046851</v>
+      </c>
+      <c r="F8">
+        <f>C8/E8</f>
+        <v>1.2472550642303637</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="F9">
+        <f>SUM(C6:C8)/SUM(E6:E8)</f>
+        <v>1.2445198557561739</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11">
+        <f>1.7/4</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12">
+        <f>5/4</f>
+        <v>1.25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13">
+        <v>1.24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="9">
+        <f>C15/((B2/20)^2*PI())</f>
+        <v>41.575168807678793</v>
+      </c>
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17">
+        <f>C15*F9</f>
+        <v>1.2445198557561739</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20">
+        <v>1.22</v>
+      </c>
+      <c r="D20">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21">
+        <v>1.21</v>
+      </c>
+      <c r="D21">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22">
+        <v>1.24</v>
+      </c>
+      <c r="D22">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <v>1.23</v>
+      </c>
+      <c r="D23">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="D24">
+        <f>AVERAGE(D20:D23)</f>
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26">
+        <v>630</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27">
+        <f>B26/D24*C17</f>
+        <v>642.66189272654879</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>